<commit_message>
Automatische test-sync: 2025-07-23 13:57:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -738,8 +738,63 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-07-23 13:57:01</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -759,7 +814,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -767,17 +822,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -819,7 +874,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 14:03:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -793,8 +793,63 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-07-23 14:03:45</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -814,7 +869,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -822,17 +877,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -874,7 +929,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 14:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,8 +848,63 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-07-23 14:21:53</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -869,7 +924,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -877,17 +932,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -929,7 +984,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 18:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -903,8 +903,63 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-07-23 18:29:40</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -924,7 +979,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -932,17 +987,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -984,7 +1039,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 18:39:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -958,8 +958,63 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-07-23 18:39:49</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -979,7 +1034,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -987,17 +1042,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1039,7 +1094,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 21:07:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,8 +1013,63 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-07-23 21:07:23</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1034,7 +1089,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1042,17 +1097,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1094,7 +1149,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 21:14:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1068,8 +1068,63 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-07-23 21:14:43</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1089,7 +1144,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1097,17 +1152,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1149,7 +1204,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 21:26:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1123,8 +1123,63 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Testmail #1: Wat zijn jullie openingstijden?</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Openingstijden / Locatie</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank u wel voor uw interesse in onze diensten. Onze openingstijden zijn van maandag tot en met vrijdag van 9:00 tot 17:00 uur. Mocht u nog verdere vragen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-07-23 21:25:56</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1144,7 +1199,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1152,17 +1207,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1204,7 +1259,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:15:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1178,8 +1178,65 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mijn product is kapot aangekomen. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Testmail #1: Mijn product is kapot aangekomen. Kunnen jullie dit oplossen?</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Wat vervelend om te horen dat uw product kapot is aangekomen. Om dit probleem op te lossen, hebben we wat meer informatie nodig.
+Zou u ons kunnen voorzien van uw ordernummer en eventueel foto's van het beschadigde product? Op die manier kunnen we uw situatie beter begrijpen en u verder helpen met een passende oplossing.
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:15:32</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1199,7 +1256,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1207,17 +1264,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1232,7 +1289,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1262,6 +1319,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:17:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1235,8 +1235,64 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kun je 100 stuks M5-bouten bestellen voor klant Jansen?</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Testmail #2: Kun je 100 stuks M5-bouten bestellen voor klant Jansen?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je e-mail. Om de bestelling voor 100 stuks M5-bouten voor klant Jansen te plaatsen, hebben we wat meer informatie nodig. Zou je ons kunnen voorzien van de specificaties van de M5-bouten (zoals het materiaal, lengte, kopvorm, enz.) zodat we de bestelling correct kunnen verwerken?
+Als je deze informatie kunt verstrekken, zullen we ervoor zorgen dat de bestelling zo spoedig mogelijk wordt geplaatst.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:17:48</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1256,7 +1312,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1264,17 +1320,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1289,7 +1345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1329,6 +1385,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1291,8 +1291,64 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Ik heb maat M ontvangen maar ik had L besteld. Kan ik ruilen?</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Testmail #3: Ik heb maat M ontvangen maar ik had L besteld. Kan ik ruilen?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor je e-mail. Het spijt me te horen dat je de verkeerde maat hebt ontvangen. Om je zo goed mogelijk van dienst te zijn, wil ik vragen of je ons je bestelnummer en de juiste maat kunt doorgeven? Op die manier kunnen we de juiste maat voor je regelen en het omruilproces in gang zetten.
+We kijken uit naar je reactie en helpen je graag verder.
+Met vriendelijke groet,
+[Naam van het bedrijf]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:20:00</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1312,7 +1368,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1320,17 +1376,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1382,7 +1438,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:22:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$4</f>
+              <f>'Dashboard'!$A$2:$A$5</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$4</f>
+              <f>'Dashboard'!$B$2:$B$5</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1347,8 +1347,64 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Wil je deze factuur even printen en klaarleggen voor maandag?</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Testmail #4: Wil je deze factuur even printen en klaarleggen voor maandag?</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Geachte heer/mevrouw,
+Helaas kan ik u niet helpen met het printen en klaarleggen van de factuur. Ik ben een e-mailassistent en kan geen fysieke taken uitvoeren. Ik raad u aan contact op te nemen met de relevante afdeling binnen uw bedrijf om dit verzoek in behandeling te nemen.
+Met vriendelijke groet,
+[Je Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:22:32</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D13">
+  <conditionalFormatting sqref="D2:D14">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1368,7 +1424,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G13">
+  <conditionalFormatting sqref="G2:G14">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1376,17 +1432,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H13">
+  <conditionalFormatting sqref="H2:H14">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I13">
+  <conditionalFormatting sqref="I2:I14">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J13">
+  <conditionalFormatting sqref="J2:J14">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1401,7 +1457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1451,6 +1507,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Factuur / Administratie</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:24:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$5</f>
+              <f>'Dashboard'!$A$2:$A$6</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$5</f>
+              <f>'Dashboard'!$B$2:$B$6</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1403,8 +1403,63 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ik probeer in te loggen maar krijg steeds een foutmelding.</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Testmail #5: Ik probeer in te loggen maar krijg steeds een foutmelding.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor het melden van dit probleem. Om u beter van dienst te kunnen zijn, vragen wij u vriendelijk om de foutmelding die u ontvangt door te sturen, samen met uw gebruikersnaam. Zo kunnen wij het probleem nauwkeuriger onderzoeken en u een oplossing bieden.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:24:46</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D14">
+  <conditionalFormatting sqref="D2:D15">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1424,7 +1479,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G14">
+  <conditionalFormatting sqref="G2:G15">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1432,17 +1487,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14">
+  <conditionalFormatting sqref="H2:H15">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I14">
+  <conditionalFormatting sqref="I2:I15">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14">
+  <conditionalFormatting sqref="J2:J15">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1457,7 +1512,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1517,6 +1572,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>IT / Technisch probleem</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:27:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$6</f>
+              <f>'Dashboard'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$6</f>
+              <f>'Dashboard'!$B$2:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1458,8 +1458,66 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Zou jij deze offerte even naar klant X willen mailen?</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Testmail #6: Zou jij deze offerte even naar klant X willen mailen?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Bedankt voor uw e-mail. Helaas kan ik u niet helpen bij het versturen van de offerte naar klant X, aangezien ik geen toegang heb tot uw documenten of het vermogen om e-mails namens u te verzenden.
+Ik raad u aan de offerte zelf naar klant X te mailen of contact op te nemen met de verantwoordelijke persoon binnen uw organisatie die dit kan afhandelen.
+Als u nog andere vragen heeft, laat het me dan weten.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:26:57</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D15">
+  <conditionalFormatting sqref="D2:D16">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1479,7 +1537,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G15">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1487,17 +1545,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H15">
+  <conditionalFormatting sqref="H2:H16">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I15">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J15">
+  <conditionalFormatting sqref="J2:J16">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1512,7 +1570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1582,6 +1640,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Offerte / Prijsaanvraag</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:29:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1516,8 +1516,63 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Mijn bestelling is er nog steeds niet. Kunnen jullie dit nakijken?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Testmail #7: Mijn bestelling is er nog steeds niet. Kunnen jullie dit nakijken?</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw bestelling te kunnen nakijken, hebben we wat meer informatie nodig. Kunt u ons uw bestelnummer of klantgegevens doorgeven? Dan kunnen we dit voor u onderzoeken en u verder helpen.
+Met vriendelijke groet,
+[Naam van het bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:29:08</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="D2:D17">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1537,7 +1592,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G16">
+  <conditionalFormatting sqref="G2:G17">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1545,17 +1600,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="H2:H17">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I16">
+  <conditionalFormatting sqref="I2:I17">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="J2:J17">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1617,7 +1672,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:31:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$7</f>
+              <f>'Dashboard'!$A$2:$A$8</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$7</f>
+              <f>'Dashboard'!$B$2:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1571,8 +1571,66 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Kun jij een demo inplannen bij Van Dijk deze week?</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Testmail #8: Kun jij een demo inplannen bij Van Dijk deze week?</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je e-mail. Voor het inplannen van een demo bij Van Dijk deze week, vragen we je om het volgende te doen:
+- Stuur ons de beschikbare data en tijden voor de demo.
+- Geef ons wat meer informatie over de gewenste inhoud van de demo, zodat we ons goed kunnen voorbereiden.
+Zodra we deze informatie hebben ontvangen, zullen we ons best doen om een geschikte datum en tijd te vinden. 
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:31:45</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D17">
+  <conditionalFormatting sqref="D2:D18">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1592,7 +1650,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
+  <conditionalFormatting sqref="G2:G18">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1600,17 +1658,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
+  <conditionalFormatting sqref="H2:H18">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
+  <conditionalFormatting sqref="I2:I18">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
+  <conditionalFormatting sqref="J2:J18">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1625,7 +1683,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1705,6 +1763,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:34:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1629,8 +1629,63 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wanneer wordt mijn retour terugbetaald?</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Testmail #9: Wanneer wordt mijn retour terugbetaald?</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank je wel voor je bericht. Om je terugbetaling van de retourzending te kunnen verwerken, hebben wij wat meer informatie nodig. Zou je ons je bestelnummer en de naam waaronder de bestelling is geplaatst kunnen doorgeven? Zo kunnen wij dit verder voor je nakijken en je zo spoedig mogelijk van dienst zijn.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:34:02</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D18">
+  <conditionalFormatting sqref="D2:D19">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1650,7 +1705,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G18">
+  <conditionalFormatting sqref="G2:G19">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1658,17 +1713,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H19">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I18">
+  <conditionalFormatting sqref="I2:I19">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J18">
+  <conditionalFormatting sqref="J2:J19">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1720,7 +1775,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:36:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1684,8 +1684,63 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Kun jij de planning voor volgende week alvast voorbereiden?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Testmail #10: Kun jij de planning voor volgende week alvast voorbereiden?</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank je wel voor je e-mail. Ik kan zeker de planning voor volgende week voorbereiden. Zou je wat meer specifieke informatie kunnen geven over de taken en activiteiten die moeten worden ingepland? Zodra ik meer details heb, kan ik aan de slag gaan met het opstellen van de planning.
+Met vriendelijke groet,
+[Naam] [Functie]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:36:15</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D19">
+  <conditionalFormatting sqref="D2:D20">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1705,7 +1760,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G19">
+  <conditionalFormatting sqref="G2:G20">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1713,17 +1768,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H19">
+  <conditionalFormatting sqref="H2:H20">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I19">
+  <conditionalFormatting sqref="I2:I20">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J19">
+  <conditionalFormatting sqref="J2:J20">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1791,17 +1846,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Planning / Afspraak</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1811,7 +1866,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -1821,7 +1876,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Planning / Afspraak</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:38:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$8</f>
+              <f>'Dashboard'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$8</f>
+              <f>'Dashboard'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1739,8 +1739,63 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Hebben jullie een handleiding van de EcoPro-500?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Testmail #11: Hebben jullie een handleiding van de EcoPro-500?</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw interesse in de EcoPro-500. Op dit moment hebben wij geen handleiding beschikbaar voor de EcoPro-500. Echter, wij kunnen u wel voorzien van de basisinformatie over het product, zoals specificaties, functies en gebruiksinstructies. Mocht u specifieke vragen hebben of meer gedetailleerde informatie nodig hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:38:27</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D20">
+  <conditionalFormatting sqref="D2:D21">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1760,7 +1815,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G20">
+  <conditionalFormatting sqref="G2:G21">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1768,17 +1823,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H20">
+  <conditionalFormatting sqref="H2:H21">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I20">
+  <conditionalFormatting sqref="I2:I21">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J20">
+  <conditionalFormatting sqref="J2:J21">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1793,7 +1848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1883,6 +1938,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:40:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1794,8 +1794,64 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Wil je kijken of die bestelling van Van Rijn al is verzonden?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Testmail #12: Wil je kijken of die bestelling van Van Rijn al is verzonden?</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Bestelling / Levering</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Dank u voor uw e-mail. Om u beter van dienst te kunnen zijn, zouden wij graag wat meer informatie ontvangen, zoals uw bestelnummer of de naam waaronder de bestelling geplaatst is. Met deze gegevens kunnen wij controleren of de bestelling van Van Rijn al verzonden is.
+Wij zien uw reactie graag tegemoet.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:40:39</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D21">
+  <conditionalFormatting sqref="D2:D22">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1815,7 +1871,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
+  <conditionalFormatting sqref="G2:G22">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1823,17 +1879,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H21">
+  <conditionalFormatting sqref="H2:H22">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I21">
+  <conditionalFormatting sqref="I2:I22">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J21">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1895,7 +1951,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:43:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$9</f>
+              <f>'Dashboard'!$A$2:$A$10</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$9</f>
+              <f>'Dashboard'!$B$2:$B$10</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1850,8 +1850,64 @@
         </is>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Ik wil me graag aanmelden voor de nieuwsbrief.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Testmail #13: Ik wil me graag aanmelden voor de nieuwsbrief.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Dank voor uw interesse in onze nieuwsbrief! U kunt zich eenvoudig aanmelden door uw e-mailadres achter te laten op onze website of door ons een bericht te sturen met het verzoek om u toe te voegen aan de nieuwsbrieflijst. 
+Mocht u nog vragen hebben of ergens hulp bij nodig hebben, dan hoor ik dat graag.
+Met vriendelijke groet,
+[Naam van het bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:42:50</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D22">
+  <conditionalFormatting sqref="D2:D23">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1871,7 +1927,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G22">
+  <conditionalFormatting sqref="G2:G23">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1879,17 +1935,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H22">
+  <conditionalFormatting sqref="H2:H23">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I22">
+  <conditionalFormatting sqref="I2:I23">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J22">
+  <conditionalFormatting sqref="J2:J23">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1904,7 +1960,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2004,6 +2060,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Afmelding / Nieuwsbrief</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1906,8 +1906,63 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Zorg jij dat deze pallets vandaag nog klaarstaan?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Testmail #14: Zorg jij dat deze pallets vandaag nog klaarstaan?</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Planning / Afspraak</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Geachte afzender,
+Hartelijk dank voor uw e-mail. Helaas is deze e-mail niet voor ons bedoeld, aangezien wij een professionele e-mailassistent zijn en geen fysieke pallets kunnen klaarzetten. Voor verdere assistentie met betrekking tot pallets verzoek ik u vriendelijk om contact op te nemen met de desbetreffende afdeling binnen uw organisatie.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:45:05</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D23">
+  <conditionalFormatting sqref="D2:D24">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1927,7 +1982,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G23">
+  <conditionalFormatting sqref="G2:G24">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1935,17 +1990,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H23">
+  <conditionalFormatting sqref="H2:H24">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I23">
+  <conditionalFormatting sqref="I2:I24">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J23">
+  <conditionalFormatting sqref="J2:J24">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2017,7 +2072,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:47:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1961,8 +1961,67 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Ik stuur het pakket morgen terug.</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Testmail #15: Ik stuur het pakket morgen terug.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Om uw retourzending zo soepel mogelijk te laten verlopen, vragen wij u vriendelijk om het volgende te doen:
+- Vul het retourformulier in dat bij uw bestelling zat en voeg dit toe aan het pakket.
+- Stuur het pakket terug naar het volgende adres: [adres retourzending].
+- Zodra wij uw retourzending hebben ontvangen, zullen wij het verder afhandelen en u op de hoogte houden van de status van uw retour.
+Mocht u nog verdere vragen of opmerkingen hebben, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam bedrijf] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:47:16</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D24">
+  <conditionalFormatting sqref="D2:D25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1982,7 +2041,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G24">
+  <conditionalFormatting sqref="G2:G25">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1990,17 +2049,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
+  <conditionalFormatting sqref="H2:H25">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I24">
+  <conditionalFormatting sqref="I2:I25">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J24">
+  <conditionalFormatting sqref="J2:J25">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2052,7 +2111,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:49:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$10</f>
+              <f>'Dashboard'!$A$2:$A$11</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$10</f>
+              <f>'Dashboard'!$B$2:$B$11</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2020,8 +2020,63 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Kun jij dit even aan Koen doorgeven?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Testmail #16: Kun jij dit even aan Koen doorgeven?</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Geachte klant,
+Bedankt voor uw e-mail. Kunt u ons wat meer context geven over het verzoek om iets aan Koen door te geven? Op deze manier kunnen we u beter van dienst zijn en ervoor zorgen dat uw bericht correct wordt doorgestuurd.
+Met vriendelijke groet,
+[Bedrijfsnaam] E-mailassistent</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:49:28</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D25">
+  <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2041,7 +2096,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G25">
+  <conditionalFormatting sqref="G2:G26">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2049,17 +2104,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H25">
+  <conditionalFormatting sqref="H2:H26">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I25">
+  <conditionalFormatting sqref="I2:I26">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J25">
+  <conditionalFormatting sqref="J2:J26">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2074,7 +2129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2137,7 +2192,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2147,7 +2202,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2181,6 +2236,16 @@
         </is>
       </c>
       <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:52:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2075,8 +2075,65 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ik heb het verkeerde artikel ontvangen.</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Testmail #17: Ik heb het verkeerde artikel ontvangen.</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Retour / Terugbetaling</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Beste klant,
+Bedankt voor uw bericht. Het spijt me te horen dat u het verkeerde artikel heeft ontvangen. Om dit probleem op te lossen, ontvang ik graag wat meer informatie van u. Kunt u mij het ordernummer en de naam van het artikel dat u hebt ontvangen sturen? Op die manier kunnen we de situatie beter begrijpen en een passende oplossing voor u vinden.
+Alvast bedankt voor uw medewerking.
+Met vriendelijke groet,
+[Naam]
+E-mailassistent van [Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:52:04</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D27">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2096,7 +2153,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G27">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2104,17 +2161,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H27">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I27">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J27">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2166,7 +2223,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:54:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2132,8 +2132,63 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Kun je nagaan of we nog EcoPro-700 op voorraad hebben?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Testmail #18: Kun je nagaan of we nog EcoPro-700 op voorraad hebben?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Productinformatie</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Bedankt voor je bericht. Op dit moment hebben we nog EcoPro-700 op voorraad. Als je wilt bestellen, laat het ons dan weten en we helpen je graag verder.
+Met vriendelijke groet,
+[Bedrijfsnaam]</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:54:16</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D27">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2153,7 +2208,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G27">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2161,17 +2216,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H27">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I27">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J27">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2249,11 +2304,11 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Productinformatie</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -2279,7 +2334,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Productinformatie</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B9" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$11</f>
+              <f>'Dashboard'!$A$2:$A$12</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$11</f>
+              <f>'Dashboard'!$B$2:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2187,8 +2187,66 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Hoe gaan jullie om met mijn persoonsgegevens?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Testmail #19: Hoe gaan jullie om met mijn persoonsgegevens?</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Juridisch / Contract</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Beste afzender,
+Dank u voor uw interesse in onze aanpak met betrekking tot persoonsgegevens. Bij ons bedrijf hechten we veel waarde aan de bescherming van persoonlijke informatie. Wij voldoen aan alle geldende wet- en regelgeving met betrekking tot gegevensbescherming, inclusief de Algemene Verordening Gegevensbescherming (AVG).
+Mocht u nog specifieke vragen hebben over hoe wij omgaan met persoonsgegevens of als u meer details wenst te ontvangen, aarzel dan niet om contact met ons op te nemen.
+Met vriendelijke groet,
+[Naam assistent]
+Nederlandse e-mailassistent
+Bedrijfsnaam</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:56:35</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D28">
+  <conditionalFormatting sqref="D2:D29">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2208,7 +2266,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G28">
+  <conditionalFormatting sqref="G2:G29">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2216,17 +2274,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H28">
+  <conditionalFormatting sqref="H2:H29">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I28">
+  <conditionalFormatting sqref="I2:I29">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J28">
+  <conditionalFormatting sqref="J2:J29">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2241,7 +2299,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2314,7 +2372,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2324,7 +2382,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2334,7 +2392,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2358,6 +2416,16 @@
         </is>
       </c>
       <c r="B11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Juridisch / Contract</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-07-23 22:58:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-07-23.xlsx
+++ b/logs/mail_log_2025-07-23.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$12</f>
+              <f>'Dashboard'!$A$2:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$12</f>
+              <f>'Dashboard'!$B$2:$B$13</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2245,8 +2245,63 @@
         </is>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Wil jij klant Dekker even bellen over die offerte?</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>mailmind.test@zohomail.eu</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Testmail #20: Wil jij klant Dekker even bellen over die offerte?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Beste [Naam],
+Bedankt voor je bericht. Ik zal klant Dekker zo snel mogelijk bellen over de offerte.
+Met vriendelijke groet,
+[Jouw Naam]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-07-23 22:58:49</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D29">
+  <conditionalFormatting sqref="D2:D30">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -2266,7 +2321,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G29">
+  <conditionalFormatting sqref="G2:G30">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2274,17 +2329,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H29">
+  <conditionalFormatting sqref="H2:H30">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I29">
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J29">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -2299,7 +2354,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2372,7 +2427,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT / Technisch probleem</t>
+          <t>Factuur / Administratie</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2382,7 +2437,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Factuur / Administratie</t>
+          <t>Offerte / Prijsaanvraag</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2392,7 +2447,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Offerte / Prijsaanvraag</t>
+          <t>IT / Technisch probleem</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2426,6 +2481,16 @@
         </is>
       </c>
       <c r="B12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Samenwerking / Partnerverzoek</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>